<commit_message>
houses in house_dict, sites into sites_dict, neigh_sites into neigh_sites_dict. sites_utils script, house_utils script, site_object and house_object
</commit_message>
<xml_diff>
--- a/house_lists.xlsx
+++ b/house_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukecoburn/AndrewBashorum_4thYearProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179B978C-6872-E147-9365-F8C9AE83C0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585F1CD7-F2A9-664B-B223-4C0D293CEA7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21240" activeTab="1" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21240" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
   </bookViews>
   <sheets>
     <sheet name="LynmouthDriveOdd" sheetId="1" r:id="rId1"/>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A86ED2D-66BF-B94F-9B04-A18B1852EAE4}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -850,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F20FAA8-FD9E-B740-B000-A9366EDC2A09}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Merging Lukes branch, added BemptonDriveEven and odd pickles and exel sheets
</commit_message>
<xml_diff>
--- a/house_lists.xlsx
+++ b/house_lists.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukecoburn/AndrewBashorum_4thYearProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbashorm/4thYearProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B806A1-C53C-B145-8F54-6452415F25E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BC1516-E981-4F44-83FB-3DAC672A4A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21240" activeTab="1" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
+    <workbookView xWindow="2000" yWindow="500" windowWidth="10000" windowHeight="19980" firstSheet="1" activeTab="1" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
   </bookViews>
   <sheets>
     <sheet name="LynmouthDriveOdd" sheetId="1" r:id="rId1"/>
-    <sheet name="test" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="LynmouthDriveEven" sheetId="2" r:id="rId4"/>
+    <sheet name="BemptonDriveOdd" sheetId="5" r:id="rId2"/>
+    <sheet name="LynmouthDriveEven" sheetId="2" r:id="rId3"/>
+    <sheet name="BemptonDriveEven" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="170">
   <si>
     <t>20 Lynmouth Dr Ruislip HA4 9BZ UK</t>
   </si>
@@ -277,6 +277,276 @@
   </si>
   <si>
     <t>53 Lynmouth Dr Ruislip HA4 9BY UK</t>
+  </si>
+  <si>
+    <t>2 Bempton Dr Ruislip HA4 9DD, UK</t>
+  </si>
+  <si>
+    <t>4 Bempton Dr Ruislip HA4 9DA, UK</t>
+  </si>
+  <si>
+    <t>6 Bempton Dr Ruislip HA4 9DA UK</t>
+  </si>
+  <si>
+    <t>8 Bempton Dr Ruislip HA4 9DA UK</t>
+  </si>
+  <si>
+    <t>10 Bempton Dr Ruislip HA4 9DA UK</t>
+  </si>
+  <si>
+    <t>12 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>14 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>20 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 Bempton Dr Ruislip HA4 9DD UK </t>
+  </si>
+  <si>
+    <t>22 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>24 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>26 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>28 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>30 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>32 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>34 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>36 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>38 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>40 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>42 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>44 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>46 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>48 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>50 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>52 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>54 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>56 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>58 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>60 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>62 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>64 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>66 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>68 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>70 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>72 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>74 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>76 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>78 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>80 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>82 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>84 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>86 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>88 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>90 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>94 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>96 Bempton Dr Ruislip HA4 9DS UK</t>
+  </si>
+  <si>
+    <t>98 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>100 Bempton Dr Ruislip HA4 9DS UK</t>
+  </si>
+  <si>
+    <t>102 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>104 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>106 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>108 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>110 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>1 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>3 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>5 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>7 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>9 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>11 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>13 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>15 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>17 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>19 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>21 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>23 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>25 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>27 Bempton Dr Ruislip HA4 9DD UK</t>
+  </si>
+  <si>
+    <t>29 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>31 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>33 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>35 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>37 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>39 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>41 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>43 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>45 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>47 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>49 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>51 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>53 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>55 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>59 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>57 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>61 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>63 Bempton Dr Ruislip HA4 9DB UK</t>
+  </si>
+  <si>
+    <t>67 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>65 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>69 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>71 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>73 Bempton Dr Ruislip HA4 9DE UK</t>
   </si>
 </sst>
 </file>
@@ -631,12 +901,12 @@
   <dimension ref="A1:A40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -849,26 +1119,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4A65FC-C706-4342-8C00-ECA1E2791449}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDB4C3C-1745-D843-877E-25D3CD1AAE66}">
+  <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -877,39 +1322,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF12F9A7-034B-824D-9F69-B3355A3A01B3}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F20FAA8-FD9E-B740-B000-A9366EDC2A09}">
   <dimension ref="A1:A40"/>
   <sheetViews>
@@ -1125,4 +1537,292 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7D77F1-CA1A-D145-91A8-C840987BA76D}">
+  <dimension ref="A1:A54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="41" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added cookie cutter function to site_finder.py
</commit_message>
<xml_diff>
--- a/house_lists.xlsx
+++ b/house_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbashorm/4thYearProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BC1516-E981-4F44-83FB-3DAC672A4A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1531F61-0163-4A42-8DF0-7CD6F8945CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="500" windowWidth="10000" windowHeight="19980" firstSheet="1" activeTab="1" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
+    <workbookView xWindow="16180" yWindow="760" windowWidth="10000" windowHeight="19980" firstSheet="2" activeTab="2" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
   </bookViews>
   <sheets>
     <sheet name="LynmouthDriveOdd" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
   <si>
     <t>20 Lynmouth Dr Ruislip HA4 9BZ UK</t>
   </si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>78 Lynmouth Dr Ruislip HA4 9BY UK</t>
-  </si>
-  <si>
-    <t>80 Lynmouth Dr Ruislip HA4 9BY UK</t>
   </si>
   <si>
     <t>51 Lynmouth Dr Ruislip HA4 9BY UK</t>
@@ -1037,12 +1034,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
@@ -1122,7 +1119,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EDB4C3C-1745-D843-877E-25D3CD1AAE66}">
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -1133,187 +1130,187 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1323,10 +1320,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F20FAA8-FD9E-B740-B000-A9366EDC2A09}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1527,11 +1524,6 @@
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1554,272 +1546,272 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cookie cutter worked on further, All dicts placed into one, more dicts added
</commit_message>
<xml_diff>
--- a/house_lists.xlsx
+++ b/house_lists.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbashorm/4thYearProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1531F61-0163-4A42-8DF0-7CD6F8945CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA6A41E-9EA9-B74E-B5F5-236F0315AE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16180" yWindow="760" windowWidth="10000" windowHeight="19980" firstSheet="2" activeTab="2" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
+    <workbookView xWindow="26740" yWindow="620" windowWidth="10000" windowHeight="19980" firstSheet="4" activeTab="5" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
   </bookViews>
   <sheets>
     <sheet name="LynmouthDriveOdd" sheetId="1" r:id="rId1"/>
     <sheet name="BemptonDriveOdd" sheetId="5" r:id="rId2"/>
     <sheet name="LynmouthDriveEven" sheetId="2" r:id="rId3"/>
     <sheet name="BemptonDriveEven" sheetId="6" r:id="rId4"/>
+    <sheet name="BeverleyRoadEven" sheetId="7" r:id="rId5"/>
+    <sheet name="BeverleyRoadOdd" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="254">
   <si>
     <t>20 Lynmouth Dr Ruislip HA4 9BZ UK</t>
   </si>
@@ -544,6 +546,261 @@
   </si>
   <si>
     <t>73 Bempton Dr Ruislip HA4 9DE UK</t>
+  </si>
+  <si>
+    <t>62 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>64 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>66 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>68 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>70 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>72 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>74 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>76 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>78 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>80 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>82 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>84 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>86 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>88 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>90 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>92 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>94 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>96 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>98 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>100 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>102 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>104 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>106 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>108 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>110 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>112 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>114 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>116 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>118 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>120 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>122 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>124 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>126 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>128 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>130 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>132 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>134 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>136 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>211 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>145 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>137 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>135 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>127 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>129 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>131 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>133 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>139 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>141 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>143 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>147 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>149 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>151 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>153 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>155 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>157 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>159 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>161 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>163 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>165 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>167 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>169 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>171 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>173 Beverley Rd Ruislip HA4 9AS UK</t>
+  </si>
+  <si>
+    <t>175 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>177 Beverley Rd Ruislip HA4 9AP UK</t>
+  </si>
+  <si>
+    <t>219 Beverley Rd Ruislip HA4 9DT UK</t>
+  </si>
+  <si>
+    <t>217 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>215 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>213 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>209 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>207 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>205 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>203 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>201 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>199 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>197 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>195 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>193 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>191 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>189 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>187 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>185 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>183 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>181 Beverley Rd Ruislip HA4 9AR UK</t>
+  </si>
+  <si>
+    <t>179 Beverley Rd Ruislip HA4 9AR UK</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1377,7 @@
   <dimension ref="A1:A37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,7 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F20FAA8-FD9E-B740-B000-A9366EDC2A09}">
   <dimension ref="A1:A39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1817,4 +2074,465 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F02AE15-5F09-EE43-B7BA-1061DB215287}">
+  <dimension ref="A1:A38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52E922F-F67F-DA40-9B7E-2B6B76BD10AE}">
+  <dimension ref="A1:A47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cookie cutter now saving raster image and vector values
</commit_message>
<xml_diff>
--- a/house_lists.xlsx
+++ b/house_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbashorm/4thYearProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AA6A41E-9EA9-B74E-B5F5-236F0315AE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B94F4A-E1C2-9749-80CC-10F168883DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26740" yWindow="620" windowWidth="10000" windowHeight="19980" firstSheet="4" activeTab="5" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
+    <workbookView xWindow="26740" yWindow="500" windowWidth="10000" windowHeight="19980" firstSheet="4" activeTab="4" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
   </bookViews>
   <sheets>
     <sheet name="LynmouthDriveOdd" sheetId="1" r:id="rId1"/>
@@ -2080,9 +2080,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F02AE15-5F09-EE43-B7BA-1061DB215287}">
   <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2288,7 +2286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52E922F-F67F-DA40-9B7E-2B6B76BD10AE}">
   <dimension ref="A1:A47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
create main autoprocessing script
</commit_message>
<xml_diff>
--- a/house_lists.xlsx
+++ b/house_lists.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukecoburn/AndrewBashorum_4thYearProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B806A1-C53C-B145-8F54-6452415F25E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D00C9D7-B48B-8B48-BB5C-E8F2FA4D0D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21240" activeTab="1" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21220" activeTab="1" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
   </bookViews>
   <sheets>
     <sheet name="LynmouthDriveOdd" sheetId="1" r:id="rId1"/>
-    <sheet name="test" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
-    <sheet name="LynmouthDriveEven" sheetId="2" r:id="rId4"/>
+    <sheet name="LynmouthDriveEven" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>20 Lynmouth Dr Ruislip HA4 9BZ UK</t>
   </si>
@@ -247,12 +245,6 @@
   </si>
   <si>
     <t>75 Lynmouth Dr Ruislip HA4 9BY UK</t>
-  </si>
-  <si>
-    <t>77 Lynmouth Dr Ruislip HA4 9BY UK</t>
-  </si>
-  <si>
-    <t>79 Lynmouth Dr Ruislip HA4 9BY UK</t>
   </si>
   <si>
     <t>70 Lynmouth Dr Ruislip HA4 9BY UK</t>
@@ -628,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A86ED2D-66BF-B94F-9B04-A18B1852EAE4}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:A6"/>
+      <selection activeCell="A39" activeCellId="1" sqref="A40 A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,12 +759,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
@@ -828,16 +820,6 @@
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -849,71 +831,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4A65FC-C706-4342-8C00-ECA1E2791449}">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF12F9A7-034B-824D-9F69-B3355A3A01B3}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F20FAA8-FD9E-B740-B000-A9366EDC2A09}">
   <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:A40"/>
     </sheetView>
   </sheetViews>
@@ -1094,32 +1015,32 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Plotter class which can plot single house single street or entire street
</commit_message>
<xml_diff>
--- a/house_lists.xlsx
+++ b/house_lists.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewbashorm/4thYearProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B94F4A-E1C2-9749-80CC-10F168883DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97C0AFB-CB4E-5F43-88D7-1376E901C6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26740" yWindow="500" windowWidth="10000" windowHeight="19980" firstSheet="4" activeTab="4" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
+    <workbookView xWindow="26740" yWindow="500" windowWidth="10000" windowHeight="19980" xr2:uid="{478285CA-865F-A047-B824-514C77E582EC}"/>
   </bookViews>
   <sheets>
     <sheet name="LynmouthDriveOdd" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="252">
   <si>
     <t>20 Lynmouth Dr Ruislip HA4 9BZ UK</t>
   </si>
@@ -249,12 +249,6 @@
   </si>
   <si>
     <t>75 Lynmouth Dr Ruislip HA4 9BY UK</t>
-  </si>
-  <si>
-    <t>77 Lynmouth Dr Ruislip HA4 9BY UK</t>
-  </si>
-  <si>
-    <t>79 Lynmouth Dr Ruislip HA4 9BY UK</t>
   </si>
   <si>
     <t>70 Lynmouth Dr Ruislip HA4 9BY UK</t>
@@ -1152,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A86ED2D-66BF-B94F-9B04-A18B1852EAE4}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1291,12 +1285,12 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
@@ -1352,16 +1346,6 @@
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1387,187 +1371,187 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -1580,7 +1564,7 @@
   <dimension ref="A1:A39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1760,27 +1744,27 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1803,272 +1787,272 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2080,7 +2064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F02AE15-5F09-EE43-B7BA-1061DB215287}">
   <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2089,192 +2073,192 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2297,237 +2281,237 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>